<commit_message>
added comments | supports authors, contributors, last updated by/date | if any objective is null, don't print
</commit_message>
<xml_diff>
--- a/sprint-excel.xlsx
+++ b/sprint-excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckalsari/Desktop/python-script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckalsari/Documents/sprints-structure-generator-script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45809A00-F3B7-B240-8129-7A8406BCACB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C2E412-C035-6B46-A966-B9489DFF4590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="2220" windowWidth="18840" windowHeight="15500" xr2:uid="{2206DC74-34CE-3D4A-A097-82782E0119D4}"/>
+    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" xr2:uid="{2206DC74-34CE-3D4A-A097-82782E0119D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Lab Title</t>
   </si>
@@ -122,9 +122,6 @@
     <t>This lab explains how to create a scheduled search detection rule.</t>
   </si>
   <si>
-    <t>Estimated Time</t>
-  </si>
-  <si>
     <t>Objective 1</t>
   </si>
   <si>
@@ -152,58 +149,113 @@
     <t>Trigger an ingest time detection rule</t>
   </si>
   <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>f</t>
+    <t>Estimated Time (in mins)</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Contributors</t>
+  </si>
+  <si>
+    <t>Last Updated Date</t>
+  </si>
+  <si>
+    <t>Last Updated By</t>
+  </si>
+  <si>
+    <t>Chintan Kalsaria, OCI Logging Analytics</t>
+  </si>
+  <si>
+    <t>Chintan Kalsaria, Kiran Palukuri, Ashish Gor, Kumar Varun, OCI Logging Analytics</t>
+  </si>
+  <si>
+    <t>Chintan Kalsaria</t>
+  </si>
+  <si>
+    <t>Navigate to Log Explorer</t>
+  </si>
+  <si>
+    <t>User interfaces of Log Explorer</t>
+  </si>
+  <si>
+    <t>Finding distribution, trends of fields and group-by</t>
+  </si>
+  <si>
+    <t>Navigate to Add Data page from Compass or Administration</t>
+  </si>
+  <si>
+    <t>Ingest logs using Service Connector</t>
+  </si>
+  <si>
+    <t>Ingest logs using Management Agent</t>
+  </si>
+  <si>
+    <t>Ingest logs from computer desktop</t>
+  </si>
+  <si>
+    <t>Create a single-line parser</t>
+  </si>
+  <si>
+    <t>Create a source</t>
+  </si>
+  <si>
+    <t>Navigate to Detection Rules</t>
+  </si>
+  <si>
+    <t>Create Scheduled Search Detection Rule</t>
+  </si>
+  <si>
+    <t>Oswaldo Osuna, Logging Analytics Development Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kumar Varun, Logging Analytics Product Management - Kiran Palukuri, Logging Analytics Product Management - Vikram Reddy, Logging Analytics Development Team </t>
+  </si>
+  <si>
+    <t>Oswaldo Osuna</t>
+  </si>
+  <si>
+    <t>Dec 18 2023</t>
+  </si>
+  <si>
+    <t>Ayoub BELMEHDI, OCI Logging Analytics</t>
+  </si>
+  <si>
+    <t>Ashish GOR, Kiran PALUKURI, Vikram REDDY, Kumar VARUN, Jolly KUNDU, OCI Logging Analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ayoub BELMEHDI</t>
+  </si>
+  <si>
+    <t>October 2023</t>
+  </si>
+  <si>
+    <t>Dec 23</t>
+  </si>
+  <si>
+    <t>Oct 23</t>
+  </si>
+  <si>
+    <t>Jan 24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -227,8 +279,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34F4058-1100-4D4D-8CBF-93F9FCB9B29C}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,15 +632,19 @@
     <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.6640625" customWidth="1"/>
+    <col min="8" max="8" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="135.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -593,29 +654,41 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -632,22 +705,28 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -661,25 +740,34 @@
         <v>21</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N3" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -693,25 +781,22 @@
         <v>22</v>
       </c>
       <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -725,25 +810,25 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -757,25 +842,25 @@
         <v>24</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -789,25 +874,22 @@
         <v>25</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="K7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -821,22 +903,37 @@
         <v>26</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
         <v>33</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" t="s">
         <v>34</v>
       </c>
-      <c r="I8" t="s">
-        <v>35</v>
-      </c>
       <c r="J8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -850,23 +947,50 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" t="s">
-        <v>51</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="K9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. generate/not generate sprint column 2. each objective have instructions, count of image, codesnippet 3. comments added 4. if sprints are added at end of excel and script runs, it will update new sprints into existing oandm folder 5. videolinks in comment
</commit_message>
<xml_diff>
--- a/sprint-excel.xlsx
+++ b/sprint-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckalsari/Documents/sprints-structure-generator-script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C2E412-C035-6B46-A966-B9489DFF4590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621566A0-3B1B-4045-866A-01BE6186DBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" xr2:uid="{2206DC74-34CE-3D4A-A097-82782E0119D4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17120" xr2:uid="{2206DC74-34CE-3D4A-A097-82782E0119D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
   <si>
     <t>Lab Title</t>
   </si>
@@ -122,30 +122,12 @@
     <t>This lab explains how to create a scheduled search detection rule.</t>
   </si>
   <si>
-    <t>Objective 1</t>
-  </si>
-  <si>
-    <t>Objective 2</t>
-  </si>
-  <si>
-    <t>Objective 3</t>
-  </si>
-  <si>
-    <t>Objective 4</t>
-  </si>
-  <si>
     <t>Check the policies</t>
   </si>
   <si>
     <t>Create an ingest time detection rule</t>
   </si>
   <si>
-    <t>Upload a file</t>
-  </si>
-  <si>
-    <t>Objective 5</t>
-  </si>
-  <si>
     <t>Trigger an ingest time detection rule</t>
   </si>
   <si>
@@ -191,9 +173,6 @@
     <t>Ingest logs using Management Agent</t>
   </si>
   <si>
-    <t>Ingest logs from computer desktop</t>
-  </si>
-  <si>
     <t>Create a single-line parser</t>
   </si>
   <si>
@@ -230,20 +209,119 @@
     <t>October 2023</t>
   </si>
   <si>
-    <t>Dec 23</t>
-  </si>
-  <si>
-    <t>Oct 23</t>
-  </si>
-  <si>
-    <t>Jan 24</t>
+    <t>Dec 2023</t>
+  </si>
+  <si>
+    <t>Oct 2023</t>
+  </si>
+  <si>
+    <t>Jan 2024</t>
+  </si>
+  <si>
+    <t>Step1</t>
+  </si>
+  <si>
+    <t>Step1_instructions</t>
+  </si>
+  <si>
+    <t>Step1_CodeSnippet</t>
+  </si>
+  <si>
+    <t>Step1_Images (count)</t>
+  </si>
+  <si>
+    <t>Step2</t>
+  </si>
+  <si>
+    <t>Step2_instructions</t>
+  </si>
+  <si>
+    <t>Step2_Images (count)</t>
+  </si>
+  <si>
+    <t>Step3</t>
+  </si>
+  <si>
+    <t>Step3_instructions</t>
+  </si>
+  <si>
+    <t>Step3_Images (count)</t>
+  </si>
+  <si>
+    <t>Step3_CodeSnippet</t>
+  </si>
+  <si>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>Step4_instructions</t>
+  </si>
+  <si>
+    <t>Step4_Images (count)</t>
+  </si>
+  <si>
+    <t>Step4_CodeSnippet</t>
+  </si>
+  <si>
+    <t>Step5</t>
+  </si>
+  <si>
+    <t>Step5_instructions</t>
+  </si>
+  <si>
+    <t>Step5_CodeSnippet</t>
+  </si>
+  <si>
+    <t>Step5_Images (count)</t>
+  </si>
+  <si>
+    <t>Step1_instructions are here</t>
+  </si>
+  <si>
+    <t>cd chintanKalsaria; mdkir chintanKalsaria</t>
+  </si>
+  <si>
+    <t>Step2_CodeSnippet</t>
+  </si>
+  <si>
+    <t>rm -rf chintanKalsaria</t>
+  </si>
+  <si>
+    <t>Step2 instructions are to be types here</t>
+  </si>
+  <si>
+    <t>Step3 instructions pls</t>
+  </si>
+  <si>
+    <t>Generate Sprint (Yes/No)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Chintan How to create a scheduled search detection rule?</t>
+  </si>
+  <si>
+    <t>Chintan How to create and trigger a ingest time detection rule?</t>
+  </si>
+  <si>
+    <t>Chintan Create a Scheduled Search Detection Rule</t>
+  </si>
+  <si>
+    <t>Chintan Create and Trigger a Ingest Time Detection Rule</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>dsf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -255,6 +333,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -279,13 +364,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,377 +709,571 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34F4058-1100-4D4D-8CBF-93F9FCB9B29C}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" customWidth="1"/>
-    <col min="6" max="6" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.6640625" customWidth="1"/>
-    <col min="8" max="8" width="41.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="135.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="49.33203125" customWidth="1"/>
+    <col min="11" max="11" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="135.1640625" customWidth="1"/>
+    <col min="17" max="18" width="24.6640625" customWidth="1"/>
+    <col min="19" max="19" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>82</v>
+      </c>
+      <c r="S2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" t="s">
+        <v>92</v>
+      </c>
+      <c r="X2">
+        <v>4</v>
+      </c>
+      <c r="Y2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>38</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="K3" t="s">
         <v>42</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="K4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="Q4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
-        <v>52</v>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
-        <v>53</v>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>5</v>
       </c>
-      <c r="K7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" t="s">
-        <v>61</v>
-      </c>
-      <c r="M7" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>10</v>
       </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="O8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
+        <v>46</v>
+      </c>
+      <c r="S8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" t="s">
-        <v>57</v>
-      </c>
-      <c r="M9" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N17" s="3"/>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S12" s="3"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S13" s="3"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>